<commit_message>
graph update, png update 0802
</commit_message>
<xml_diff>
--- a/RT_predict_confirm.xlsx
+++ b/RT_predict_confirm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eunwoo\PycharmProjects\RTPredict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB79469-D205-4699-A833-47FB9DA73BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109D0C99-8D30-4C0D-85D2-8F4E8B1EB26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34350" yWindow="375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RT_predict_confirm - 복사본" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>CN(C)C1=C(C=CC=C2S(=O)(OC3=CC=C(CC(O)=O)C=C3)=O)C2=CC=C1</t>
   </si>
   <si>
-    <t>CN(C)C1=C(C=CC=C2S(=O)(NC(C(O)=O)CC3=CC(I)=C(OS(O)(C4=CC=CC5=C(N(C)C)C=CC=C54)=O)C=C3)=O)C2=CC=C1</t>
-  </si>
-  <si>
     <t>CN(C)C1=C(C=CC=C2S(=O)(NCCC3=CC(OC)=C(C=C3)OS(C4=CC=CC5=C(N(C)C)C=CC=C54)(=O)=O)=O)C2=CC=C1</t>
   </si>
   <si>
@@ -1122,6 +1119,10 @@
   </si>
   <si>
     <t>RMSE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>O=C(O)C(NS(C1=C2C(C(N(C)C)=CC=C2)=CC=C1)(=O)=O)CC3=CC(I)=C(OS(C4=C5C(C(N(C)C)=CC=C5)=CC=C4)(=O)=O)C=C3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2141,32 +2142,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G316"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
+      <selection activeCell="I293" sqref="I293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" t="s">
         <v>316</v>
       </c>
-      <c r="C1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D1" t="s">
-        <v>317</v>
-      </c>
       <c r="E1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2">
         <v>1.1499999999999999</v>
@@ -2183,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G2">
         <f>_xlfn.QUARTILE.INC(D2:D316,1)</f>
@@ -2192,7 +2196,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3">
         <v>1.28</v>
@@ -2209,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G3">
         <f>_xlfn.QUARTILE.INC(D2:D316,3)</f>
@@ -2218,7 +2222,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4">
         <v>1.44</v>
@@ -2235,7 +2239,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G4">
         <f>G3-G2</f>
@@ -2244,7 +2248,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5">
         <v>1.48</v>
@@ -2261,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G5">
         <f>G2-(G4*1.5)</f>
@@ -2270,7 +2274,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6">
         <v>1.49</v>
@@ -2287,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G6">
         <f>G3+(G4*1.5)</f>
@@ -2296,7 +2300,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7">
         <v>1.59</v>
@@ -2315,7 +2319,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8">
         <v>1.6</v>
@@ -2334,7 +2338,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B9">
         <v>1.64</v>
@@ -2353,7 +2357,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10">
         <v>1.69</v>
@@ -2372,7 +2376,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>1.75</v>
@@ -2391,7 +2395,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12">
         <v>1.79</v>
@@ -2410,7 +2414,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1.88</v>
@@ -2429,7 +2433,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14">
         <v>2.0099999999999998</v>
@@ -2448,7 +2452,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>2.02</v>
@@ -2467,7 +2471,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>2.12</v>
@@ -2505,7 +2509,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>2.2200000000000002</v>
@@ -2524,7 +2528,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>2.2400000000000002</v>
@@ -2543,7 +2547,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20">
         <v>2.2599999999999998</v>
@@ -2562,7 +2566,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21">
         <v>2.44</v>
@@ -2581,7 +2585,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B22">
         <v>2.4700000000000002</v>
@@ -2619,7 +2623,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>2.74</v>
@@ -2638,7 +2642,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B25">
         <v>2.81</v>
@@ -2657,7 +2661,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <v>2.87</v>
@@ -2676,7 +2680,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B27">
         <v>2.94</v>
@@ -2695,7 +2699,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -2714,7 +2718,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -2733,7 +2737,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -2752,7 +2756,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31">
         <v>3.02</v>
@@ -2771,7 +2775,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B32">
         <v>3.05</v>
@@ -2790,7 +2794,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B33">
         <v>3.27</v>
@@ -2809,7 +2813,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34">
         <v>3.32</v>
@@ -2828,7 +2832,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B35">
         <v>3.32</v>
@@ -2847,7 +2851,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B36">
         <v>3.39</v>
@@ -2866,7 +2870,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B37">
         <v>3.44</v>
@@ -2885,7 +2889,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B38">
         <v>3.65</v>
@@ -2904,7 +2908,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B39">
         <v>3.72</v>
@@ -2923,7 +2927,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B40">
         <v>3.74</v>
@@ -2942,7 +2946,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B41">
         <v>3.84</v>
@@ -2961,7 +2965,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42">
         <v>3.94</v>
@@ -2980,7 +2984,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43">
         <v>4.05</v>
@@ -2999,7 +3003,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B44">
         <v>4.2</v>
@@ -3018,7 +3022,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45">
         <v>4.4000000000000004</v>
@@ -3037,7 +3041,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B46">
         <v>4.47</v>
@@ -3056,7 +3060,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B47">
         <v>4.5199999999999996</v>
@@ -3075,7 +3079,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B48">
         <v>4.58</v>
@@ -3094,7 +3098,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B49">
         <v>4.66</v>
@@ -3113,7 +3117,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B50">
         <v>5.05</v>
@@ -3132,7 +3136,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51">
         <v>5.16</v>
@@ -3151,7 +3155,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B52">
         <v>5.17</v>
@@ -3170,7 +3174,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B53">
         <v>5.49</v>
@@ -3189,7 +3193,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54">
         <v>5.57</v>
@@ -3208,7 +3212,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55">
         <v>5.65</v>
@@ -3227,7 +3231,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56">
         <v>5.71</v>
@@ -3246,7 +3250,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57">
         <v>5.79</v>
@@ -3265,7 +3269,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B58">
         <v>5.82</v>
@@ -3284,7 +3288,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B59">
         <v>5.85</v>
@@ -3303,7 +3307,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60">
         <v>5.87</v>
@@ -3322,7 +3326,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B61">
         <v>5.97</v>
@@ -3341,7 +3345,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B62">
         <v>5.98</v>
@@ -3360,7 +3364,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B63">
         <v>6</v>
@@ -3379,7 +3383,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B64">
         <v>6.03</v>
@@ -3398,7 +3402,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B65">
         <v>6.06</v>
@@ -3417,7 +3421,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B66">
         <v>6.19</v>
@@ -3436,7 +3440,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B67">
         <v>6.4</v>
@@ -3455,7 +3459,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B68">
         <v>6.59</v>
@@ -3474,7 +3478,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B69">
         <v>6.72</v>
@@ -3493,7 +3497,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B70">
         <v>6.79</v>
@@ -3512,7 +3516,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B71">
         <v>6.8</v>
@@ -3531,7 +3535,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B72">
         <v>6.97</v>
@@ -3550,7 +3554,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B73">
         <v>7.07</v>
@@ -3569,7 +3573,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B74">
         <v>7.17</v>
@@ -3588,7 +3592,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B75">
         <v>7.2</v>
@@ -3607,7 +3611,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B76">
         <v>7.24</v>
@@ -3626,7 +3630,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B77">
         <v>7.25</v>
@@ -3645,7 +3649,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B78">
         <v>7.38</v>
@@ -3664,7 +3668,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B79">
         <v>7.53</v>
@@ -3683,7 +3687,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B80">
         <v>7.57</v>
@@ -3702,7 +3706,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B81">
         <v>7.58</v>
@@ -3721,7 +3725,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B82">
         <v>7.59</v>
@@ -3740,7 +3744,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B83">
         <v>7.6</v>
@@ -3759,7 +3763,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B84">
         <v>7.68</v>
@@ -3778,7 +3782,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B85">
         <v>7.79</v>
@@ -3797,7 +3801,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B86">
         <v>7.84</v>
@@ -3816,7 +3820,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B87">
         <v>8.07</v>
@@ -3835,7 +3839,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B88">
         <v>8.27</v>
@@ -3854,7 +3858,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B89">
         <v>8.2899999999999991</v>
@@ -3873,7 +3877,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B90">
         <v>8.3699999999999992</v>
@@ -3892,7 +3896,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B91">
         <v>8.3800000000000008</v>
@@ -3911,7 +3915,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B92">
         <v>8.42</v>
@@ -3930,7 +3934,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B93">
         <v>8.49</v>
@@ -3949,7 +3953,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B94">
         <v>8.5399999999999991</v>
@@ -3968,7 +3972,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95">
         <v>8.59</v>
@@ -3987,7 +3991,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B96">
         <v>8.6199999999999992</v>
@@ -4006,7 +4010,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B97">
         <v>8.67</v>
@@ -4025,7 +4029,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B98">
         <v>8.67</v>
@@ -4044,7 +4048,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B99">
         <v>8.68</v>
@@ -4063,7 +4067,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B100">
         <v>8.7200000000000006</v>
@@ -4082,7 +4086,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B101">
         <v>8.73</v>
@@ -4101,7 +4105,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B102">
         <v>8.73</v>
@@ -4120,7 +4124,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B103">
         <v>8.8699999999999992</v>
@@ -4139,7 +4143,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B104">
         <v>8.9</v>
@@ -4158,7 +4162,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B105">
         <v>8.91</v>
@@ -4177,7 +4181,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B106">
         <v>8.9499999999999993</v>
@@ -4196,7 +4200,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B107">
         <v>8.9499999999999993</v>
@@ -4215,7 +4219,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B108">
         <v>9.06</v>
@@ -4234,7 +4238,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B109">
         <v>9.1300000000000008</v>
@@ -4253,7 +4257,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B110">
         <v>9.19</v>
@@ -4272,7 +4276,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B111">
         <v>9.23</v>
@@ -4291,7 +4295,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B112">
         <v>9.26</v>
@@ -4310,7 +4314,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B113">
         <v>9.34</v>
@@ -4329,7 +4333,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B114">
         <v>9.3699999999999992</v>
@@ -4348,7 +4352,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B115">
         <v>9.3800000000000008</v>
@@ -4367,7 +4371,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B116">
         <v>9.39</v>
@@ -4386,7 +4390,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B117">
         <v>9.43</v>
@@ -4405,7 +4409,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B118">
         <v>9.4600000000000009</v>
@@ -4424,7 +4428,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B119">
         <v>9.51</v>
@@ -4443,7 +4447,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B120">
         <v>9.5500000000000007</v>
@@ -4462,7 +4466,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B121">
         <v>9.57</v>
@@ -4481,7 +4485,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B122">
         <v>9.65</v>
@@ -4500,7 +4504,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B123">
         <v>9.7899999999999991</v>
@@ -4519,7 +4523,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B124">
         <v>9.82</v>
@@ -4538,7 +4542,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B125">
         <v>10.07</v>
@@ -4557,7 +4561,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B126">
         <v>10.119999999999999</v>
@@ -4576,7 +4580,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B127">
         <v>10.14</v>
@@ -4595,7 +4599,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B128">
         <v>10.18</v>
@@ -4614,7 +4618,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B129">
         <v>10.18</v>
@@ -4633,7 +4637,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B130">
         <v>10.210000000000001</v>
@@ -4652,7 +4656,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B131">
         <v>10.32</v>
@@ -4671,7 +4675,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B132">
         <v>10.52</v>
@@ -4690,7 +4694,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B133">
         <v>10.54</v>
@@ -4709,7 +4713,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B134">
         <v>10.58</v>
@@ -4728,7 +4732,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B135">
         <v>10.77</v>
@@ -4747,7 +4751,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B136">
         <v>10.78</v>
@@ -4766,7 +4770,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B137">
         <v>10.78</v>
@@ -4785,7 +4789,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B138">
         <v>10.81</v>
@@ -4804,7 +4808,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B139">
         <v>10.82</v>
@@ -4823,7 +4827,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B140">
         <v>10.89</v>
@@ -4842,7 +4846,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B141">
         <v>11</v>
@@ -4861,7 +4865,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B142">
         <v>11.05</v>
@@ -4880,7 +4884,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B143">
         <v>11.09</v>
@@ -4899,7 +4903,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B144">
         <v>11.12</v>
@@ -4918,7 +4922,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B145">
         <v>11.19</v>
@@ -4937,7 +4941,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B146">
         <v>11.22</v>
@@ -4956,7 +4960,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B147">
         <v>11.34</v>
@@ -4975,7 +4979,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B148">
         <v>11.36</v>
@@ -4994,7 +4998,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B149">
         <v>11.36</v>
@@ -5013,7 +5017,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B150">
         <v>11.37</v>
@@ -5032,7 +5036,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B151">
         <v>11.44</v>
@@ -5051,7 +5055,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B152">
         <v>11.44</v>
@@ -5070,7 +5074,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B153">
         <v>11.52</v>
@@ -5089,7 +5093,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B154">
         <v>11.59</v>
@@ -5108,7 +5112,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B155">
         <v>11.65</v>
@@ -5127,7 +5131,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B156">
         <v>11.69</v>
@@ -5146,7 +5150,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B157">
         <v>11.76</v>
@@ -5165,7 +5169,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B158">
         <v>11.82</v>
@@ -5184,7 +5188,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B159">
         <v>11.91</v>
@@ -5203,7 +5207,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B160">
         <v>11.97</v>
@@ -5222,7 +5226,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B161">
         <v>12.01</v>
@@ -5241,7 +5245,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B162">
         <v>12.02</v>
@@ -5260,7 +5264,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B163">
         <v>12.11</v>
@@ -5279,7 +5283,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B164">
         <v>12.21</v>
@@ -5298,7 +5302,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B165">
         <v>12.22</v>
@@ -5317,7 +5321,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B166">
         <v>12.22</v>
@@ -5336,7 +5340,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B167">
         <v>12.3</v>
@@ -5355,7 +5359,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B168">
         <v>12.74</v>
@@ -5374,7 +5378,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B169">
         <v>12.74</v>
@@ -5393,7 +5397,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B170">
         <v>12.81</v>
@@ -5412,7 +5416,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B171">
         <v>12.94</v>
@@ -5431,7 +5435,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B172">
         <v>12.96</v>
@@ -5450,7 +5454,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B173">
         <v>12.99</v>
@@ -5469,7 +5473,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B174">
         <v>13.06</v>
@@ -5488,7 +5492,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B175">
         <v>13.13</v>
@@ -5507,7 +5511,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B176">
         <v>13.2</v>
@@ -5526,7 +5530,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B177">
         <v>13.21</v>
@@ -5545,7 +5549,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B178">
         <v>13.23</v>
@@ -5564,7 +5568,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B179">
         <v>13.33</v>
@@ -5583,7 +5587,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B180">
         <v>13.34</v>
@@ -5602,7 +5606,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B181">
         <v>13.36</v>
@@ -5621,7 +5625,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B182">
         <v>13.45</v>
@@ -5640,7 +5644,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B183">
         <v>13.52</v>
@@ -5659,7 +5663,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B184">
         <v>13.57</v>
@@ -5678,7 +5682,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B185">
         <v>13.61</v>
@@ -5697,7 +5701,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B186">
         <v>13.61</v>
@@ -5716,7 +5720,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B187">
         <v>13.62</v>
@@ -5735,7 +5739,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B188">
         <v>13.65</v>
@@ -5754,7 +5758,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B189">
         <v>13.69</v>
@@ -5773,7 +5777,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B190">
         <v>13.72</v>
@@ -5792,7 +5796,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B191">
         <v>13.77</v>
@@ -5811,7 +5815,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B192">
         <v>13.87</v>
@@ -5830,7 +5834,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B193">
         <v>13.88</v>
@@ -5849,7 +5853,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B194">
         <v>14.11</v>
@@ -5868,7 +5872,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B195">
         <v>14.11</v>
@@ -5887,7 +5891,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B196">
         <v>14.12</v>
@@ -5906,7 +5910,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B197">
         <v>14.29</v>
@@ -5925,7 +5929,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B198">
         <v>14.32</v>
@@ -5944,7 +5948,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B199">
         <v>14.39</v>
@@ -5963,7 +5967,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B200">
         <v>14.6</v>
@@ -5982,7 +5986,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B201">
         <v>15.07</v>
@@ -6001,7 +6005,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B202">
         <v>15.08</v>
@@ -6020,7 +6024,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B203">
         <v>15.09</v>
@@ -6039,7 +6043,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B204">
         <v>15.09</v>
@@ -6058,7 +6062,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B205">
         <v>15.13</v>
@@ -6077,7 +6081,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B206">
         <v>15.28</v>
@@ -6096,7 +6100,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B207">
         <v>15.29</v>
@@ -6115,7 +6119,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B208">
         <v>15.32</v>
@@ -6134,7 +6138,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B209">
         <v>15.36</v>
@@ -6153,7 +6157,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B210">
         <v>15.42</v>
@@ -6172,7 +6176,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B211">
         <v>15.55</v>
@@ -6191,7 +6195,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B212">
         <v>15.62</v>
@@ -6210,7 +6214,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B213">
         <v>15.65</v>
@@ -6229,7 +6233,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B214">
         <v>15.69</v>
@@ -6248,7 +6252,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B215">
         <v>15.77</v>
@@ -6267,7 +6271,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B216">
         <v>15.8</v>
@@ -6286,7 +6290,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B217">
         <v>15.82</v>
@@ -6305,7 +6309,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B218">
         <v>15.9</v>
@@ -6324,7 +6328,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B219">
         <v>16.29</v>
@@ -6343,7 +6347,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B220">
         <v>16.3</v>
@@ -6362,7 +6366,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B221">
         <v>16.309999999999999</v>
@@ -6381,7 +6385,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B222">
         <v>16.350000000000001</v>
@@ -6400,7 +6404,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B223">
         <v>16.38</v>
@@ -6419,7 +6423,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B224">
         <v>16.420000000000002</v>
@@ -6438,7 +6442,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B225">
         <v>16.510000000000002</v>
@@ -6457,7 +6461,7 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B226">
         <v>16.52</v>
@@ -6476,7 +6480,7 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B227">
         <v>16.55</v>
@@ -6495,7 +6499,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B228">
         <v>16.579999999999998</v>
@@ -6514,7 +6518,7 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B229">
         <v>16.59</v>
@@ -6533,7 +6537,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B230">
         <v>16.62</v>
@@ -6552,7 +6556,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B231">
         <v>16.690000000000001</v>
@@ -6571,7 +6575,7 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B232">
         <v>16.72</v>
@@ -6590,7 +6594,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B233">
         <v>16.8</v>
@@ -6628,7 +6632,7 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B235">
         <v>17.11</v>
@@ -6647,7 +6651,7 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B236">
         <v>17.32</v>
@@ -6666,7 +6670,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B237">
         <v>17.34</v>
@@ -6685,7 +6689,7 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B238">
         <v>17.47</v>
@@ -6704,7 +6708,7 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B239">
         <v>17.489999999999998</v>
@@ -6723,7 +6727,7 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B240">
         <v>17.57</v>
@@ -6742,7 +6746,7 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B241">
         <v>17.62</v>
@@ -6761,7 +6765,7 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B242">
         <v>18.010000000000002</v>
@@ -6780,7 +6784,7 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B243">
         <v>18.03</v>
@@ -6799,7 +6803,7 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B244">
         <v>18.04</v>
@@ -6818,7 +6822,7 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B245">
         <v>18.09</v>
@@ -6837,7 +6841,7 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B246">
         <v>18.100000000000001</v>
@@ -6856,7 +6860,7 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B247">
         <v>18.14</v>
@@ -6875,7 +6879,7 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B248">
         <v>18.47</v>
@@ -6894,7 +6898,7 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B249">
         <v>18.510000000000002</v>
@@ -6913,7 +6917,7 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B250">
         <v>18.559999999999999</v>
@@ -6932,7 +6936,7 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B251">
         <v>18.63</v>
@@ -6951,7 +6955,7 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B252">
         <v>19.14</v>
@@ -6970,7 +6974,7 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B253">
         <v>19.2</v>
@@ -6989,7 +6993,7 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B254">
         <v>19.27</v>
@@ -7008,7 +7012,7 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B255">
         <v>19.38</v>
@@ -7027,7 +7031,7 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B256">
         <v>19.43</v>
@@ -7046,7 +7050,7 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B257">
         <v>19.45</v>
@@ -7065,7 +7069,7 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B258">
         <v>19.47</v>
@@ -7084,7 +7088,7 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B259">
         <v>19.95</v>
@@ -7103,7 +7107,7 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B260">
         <v>20.079999999999998</v>
@@ -7122,7 +7126,7 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B261">
         <v>20.190000000000001</v>
@@ -7141,7 +7145,7 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B262">
         <v>20.29</v>
@@ -7160,7 +7164,7 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B263">
         <v>20.36</v>
@@ -7198,7 +7202,7 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B265">
         <v>20.61</v>
@@ -7217,7 +7221,7 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B266">
         <v>20.77</v>
@@ -7236,7 +7240,7 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B267">
         <v>20.86</v>
@@ -7255,7 +7259,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B268">
         <v>21.24</v>
@@ -7274,7 +7278,7 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B269">
         <v>21.27</v>
@@ -7293,7 +7297,7 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B270">
         <v>21.31</v>
@@ -7312,7 +7316,7 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B271">
         <v>21.63</v>
@@ -7331,7 +7335,7 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B272">
         <v>21.64</v>
@@ -7350,7 +7354,7 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B273">
         <v>21.73</v>
@@ -7369,7 +7373,7 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B274">
         <v>21.85</v>
@@ -7388,7 +7392,7 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B275">
         <v>22.09</v>
@@ -7407,7 +7411,7 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B276">
         <v>22.38</v>
@@ -7426,7 +7430,7 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B277">
         <v>22.39</v>
@@ -7445,7 +7449,7 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B278">
         <v>22.52</v>
@@ -7464,7 +7468,7 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B279">
         <v>22.54</v>
@@ -7483,7 +7487,7 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B280">
         <v>22.61</v>
@@ -7502,7 +7506,7 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B281">
         <v>22.61</v>
@@ -7521,7 +7525,7 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B282">
         <v>22.65</v>
@@ -7540,7 +7544,7 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B283">
         <v>22.83</v>
@@ -7559,7 +7563,7 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B284">
         <v>23.16</v>
@@ -7578,7 +7582,7 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B285">
         <v>23.25</v>
@@ -7597,7 +7601,7 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B286">
         <v>23.41</v>
@@ -7616,7 +7620,7 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B287">
         <v>23.45</v>
@@ -7635,7 +7639,7 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B288">
         <v>23.57</v>
@@ -7654,7 +7658,7 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B289">
         <v>23.75</v>
@@ -7673,7 +7677,7 @@
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B290">
         <v>23.77</v>
@@ -7692,7 +7696,7 @@
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>4</v>
+        <v>357</v>
       </c>
       <c r="B291">
         <v>23.88</v>
@@ -7711,7 +7715,7 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B292">
         <v>23.9</v>
@@ -7730,7 +7734,7 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B293">
         <v>23.93</v>
@@ -7749,7 +7753,7 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B294">
         <v>23.98</v>
@@ -7768,7 +7772,7 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B295">
         <v>24.1</v>
@@ -7787,7 +7791,7 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B296">
         <v>24.18</v>
@@ -7806,7 +7810,7 @@
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B297">
         <v>24.22</v>
@@ -7825,7 +7829,7 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B298">
         <v>24.44</v>
@@ -7844,7 +7848,7 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B299">
         <v>24.51</v>
@@ -7863,7 +7867,7 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B300">
         <v>24.54</v>
@@ -7882,7 +7886,7 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B301">
         <v>24.6</v>
@@ -7901,7 +7905,7 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B302">
         <v>24.64</v>
@@ -7920,7 +7924,7 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B303">
         <v>24.65</v>
@@ -7939,7 +7943,7 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B304">
         <v>24.69</v>
@@ -7958,7 +7962,7 @@
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B305">
         <v>24.84</v>
@@ -7977,7 +7981,7 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B306">
         <v>24.95</v>
@@ -7996,7 +8000,7 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B307">
         <v>25.04</v>
@@ -8015,7 +8019,7 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B308">
         <v>25.39</v>
@@ -8034,7 +8038,7 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B309">
         <v>25.44</v>
@@ -8053,7 +8057,7 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B310">
         <v>25.49</v>
@@ -8072,7 +8076,7 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B311">
         <v>25.63</v>
@@ -8091,7 +8095,7 @@
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B312">
         <v>25.83</v>
@@ -8110,7 +8114,7 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B313">
         <v>26.3</v>
@@ -8129,7 +8133,7 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B314">
         <v>26.34</v>
@@ -8148,7 +8152,7 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B315">
         <v>26.7</v>
@@ -8167,7 +8171,7 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B316">
         <v>27.74</v>
@@ -8215,10 +8219,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -10631,7 +10635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC484A4-F4B1-4211-8858-3AD160FDAD22}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -10644,19 +10648,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B4" s="1">
         <v>0.97847749700374798</v>
@@ -10664,7 +10668,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" s="1">
         <v>0.9574182121427196</v>
@@ -10672,7 +10676,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="5">
         <v>0.95727532023715833</v>
@@ -10680,7 +10684,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B7" s="1">
         <v>1.2451167561865917</v>
@@ -10688,7 +10692,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B8" s="2">
         <v>300</v>
@@ -10696,30 +10700,30 @@
     </row>
     <row r="10" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -10739,7 +10743,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B13" s="1">
         <v>298</v>
@@ -10753,7 +10757,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="H13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I13" s="6">
         <f>SQRT(D13)</f>
@@ -10762,7 +10766,7 @@
     </row>
     <row r="14" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B14" s="2">
         <v>299</v>
@@ -10778,33 +10782,33 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B17" s="1">
         <v>1.7779272265709221</v>
@@ -10833,7 +10837,7 @@
     </row>
     <row r="18" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B18" s="2">
         <v>0.86773417211758253</v>
@@ -10881,22 +10885,22 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B4" s="1">
         <v>12.57916666666666</v>
@@ -10907,7 +10911,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="1">
         <v>46.139153483835187</v>
@@ -10918,7 +10922,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B6" s="1">
         <v>300</v>
@@ -10929,7 +10933,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B7" s="1">
         <v>299</v>
@@ -10940,7 +10944,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B8" s="5">
         <v>1.2715348949042349</v>
@@ -10949,7 +10953,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B9" s="1">
         <v>1.9099334878920737E-2</v>
@@ -10958,7 +10962,7 @@
     </row>
     <row r="10" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B10" s="2">
         <v>1.209916742593254</v>

</xml_diff>

<commit_message>
graph update, png update
</commit_message>
<xml_diff>
--- a/RT_predict_confirm.xlsx
+++ b/RT_predict_confirm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eunwoo\PycharmProjects\RTPredict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB79469-D205-4699-A833-47FB9DA73BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109D0C99-8D30-4C0D-85D2-8F4E8B1EB26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34350" yWindow="375" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RT_predict_confirm - 복사본" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>CN(C)C1=C(C=CC=C2S(=O)(OC3=CC=C(CC(O)=O)C=C3)=O)C2=CC=C1</t>
   </si>
   <si>
-    <t>CN(C)C1=C(C=CC=C2S(=O)(NC(C(O)=O)CC3=CC(I)=C(OS(O)(C4=CC=CC5=C(N(C)C)C=CC=C54)=O)C=C3)=O)C2=CC=C1</t>
-  </si>
-  <si>
     <t>CN(C)C1=C(C=CC=C2S(=O)(NCCC3=CC(OC)=C(C=C3)OS(C4=CC=CC5=C(N(C)C)C=CC=C54)(=O)=O)=O)C2=CC=C1</t>
   </si>
   <si>
@@ -1122,6 +1119,10 @@
   </si>
   <si>
     <t>RMSE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>O=C(O)C(NS(C1=C2C(C(N(C)C)=CC=C2)=CC=C1)(=O)=O)CC3=CC(I)=C(OS(C4=C5C(C(N(C)C)=CC=C5)=CC=C4)(=O)=O)C=C3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2141,32 +2142,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G316"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
+      <selection activeCell="I293" sqref="I293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" t="s">
         <v>316</v>
       </c>
-      <c r="C1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D1" t="s">
-        <v>317</v>
-      </c>
       <c r="E1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2">
         <v>1.1499999999999999</v>
@@ -2183,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G2">
         <f>_xlfn.QUARTILE.INC(D2:D316,1)</f>
@@ -2192,7 +2196,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3">
         <v>1.28</v>
@@ -2209,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G3">
         <f>_xlfn.QUARTILE.INC(D2:D316,3)</f>
@@ -2218,7 +2222,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4">
         <v>1.44</v>
@@ -2235,7 +2239,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G4">
         <f>G3-G2</f>
@@ -2244,7 +2248,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5">
         <v>1.48</v>
@@ -2261,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G5">
         <f>G2-(G4*1.5)</f>
@@ -2270,7 +2274,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6">
         <v>1.49</v>
@@ -2287,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G6">
         <f>G3+(G4*1.5)</f>
@@ -2296,7 +2300,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7">
         <v>1.59</v>
@@ -2315,7 +2319,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8">
         <v>1.6</v>
@@ -2334,7 +2338,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B9">
         <v>1.64</v>
@@ -2353,7 +2357,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10">
         <v>1.69</v>
@@ -2372,7 +2376,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>1.75</v>
@@ -2391,7 +2395,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12">
         <v>1.79</v>
@@ -2410,7 +2414,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1.88</v>
@@ -2429,7 +2433,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14">
         <v>2.0099999999999998</v>
@@ -2448,7 +2452,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>2.02</v>
@@ -2467,7 +2471,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>2.12</v>
@@ -2505,7 +2509,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>2.2200000000000002</v>
@@ -2524,7 +2528,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>2.2400000000000002</v>
@@ -2543,7 +2547,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20">
         <v>2.2599999999999998</v>
@@ -2562,7 +2566,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21">
         <v>2.44</v>
@@ -2581,7 +2585,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B22">
         <v>2.4700000000000002</v>
@@ -2619,7 +2623,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>2.74</v>
@@ -2638,7 +2642,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B25">
         <v>2.81</v>
@@ -2657,7 +2661,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <v>2.87</v>
@@ -2676,7 +2680,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B27">
         <v>2.94</v>
@@ -2695,7 +2699,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -2714,7 +2718,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -2733,7 +2737,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -2752,7 +2756,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31">
         <v>3.02</v>
@@ -2771,7 +2775,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B32">
         <v>3.05</v>
@@ -2790,7 +2794,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B33">
         <v>3.27</v>
@@ -2809,7 +2813,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34">
         <v>3.32</v>
@@ -2828,7 +2832,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B35">
         <v>3.32</v>
@@ -2847,7 +2851,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B36">
         <v>3.39</v>
@@ -2866,7 +2870,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B37">
         <v>3.44</v>
@@ -2885,7 +2889,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B38">
         <v>3.65</v>
@@ -2904,7 +2908,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B39">
         <v>3.72</v>
@@ -2923,7 +2927,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B40">
         <v>3.74</v>
@@ -2942,7 +2946,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B41">
         <v>3.84</v>
@@ -2961,7 +2965,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42">
         <v>3.94</v>
@@ -2980,7 +2984,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43">
         <v>4.05</v>
@@ -2999,7 +3003,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B44">
         <v>4.2</v>
@@ -3018,7 +3022,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45">
         <v>4.4000000000000004</v>
@@ -3037,7 +3041,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B46">
         <v>4.47</v>
@@ -3056,7 +3060,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B47">
         <v>4.5199999999999996</v>
@@ -3075,7 +3079,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B48">
         <v>4.58</v>
@@ -3094,7 +3098,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B49">
         <v>4.66</v>
@@ -3113,7 +3117,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B50">
         <v>5.05</v>
@@ -3132,7 +3136,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51">
         <v>5.16</v>
@@ -3151,7 +3155,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B52">
         <v>5.17</v>
@@ -3170,7 +3174,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B53">
         <v>5.49</v>
@@ -3189,7 +3193,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54">
         <v>5.57</v>
@@ -3208,7 +3212,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55">
         <v>5.65</v>
@@ -3227,7 +3231,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56">
         <v>5.71</v>
@@ -3246,7 +3250,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57">
         <v>5.79</v>
@@ -3265,7 +3269,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B58">
         <v>5.82</v>
@@ -3284,7 +3288,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B59">
         <v>5.85</v>
@@ -3303,7 +3307,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60">
         <v>5.87</v>
@@ -3322,7 +3326,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B61">
         <v>5.97</v>
@@ -3341,7 +3345,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B62">
         <v>5.98</v>
@@ -3360,7 +3364,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B63">
         <v>6</v>
@@ -3379,7 +3383,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B64">
         <v>6.03</v>
@@ -3398,7 +3402,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B65">
         <v>6.06</v>
@@ -3417,7 +3421,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B66">
         <v>6.19</v>
@@ -3436,7 +3440,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B67">
         <v>6.4</v>
@@ -3455,7 +3459,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B68">
         <v>6.59</v>
@@ -3474,7 +3478,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B69">
         <v>6.72</v>
@@ -3493,7 +3497,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B70">
         <v>6.79</v>
@@ -3512,7 +3516,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B71">
         <v>6.8</v>
@@ -3531,7 +3535,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B72">
         <v>6.97</v>
@@ -3550,7 +3554,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B73">
         <v>7.07</v>
@@ -3569,7 +3573,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B74">
         <v>7.17</v>
@@ -3588,7 +3592,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B75">
         <v>7.2</v>
@@ -3607,7 +3611,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B76">
         <v>7.24</v>
@@ -3626,7 +3630,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B77">
         <v>7.25</v>
@@ -3645,7 +3649,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B78">
         <v>7.38</v>
@@ -3664,7 +3668,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B79">
         <v>7.53</v>
@@ -3683,7 +3687,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B80">
         <v>7.57</v>
@@ -3702,7 +3706,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B81">
         <v>7.58</v>
@@ -3721,7 +3725,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B82">
         <v>7.59</v>
@@ -3740,7 +3744,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B83">
         <v>7.6</v>
@@ -3759,7 +3763,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B84">
         <v>7.68</v>
@@ -3778,7 +3782,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B85">
         <v>7.79</v>
@@ -3797,7 +3801,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B86">
         <v>7.84</v>
@@ -3816,7 +3820,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B87">
         <v>8.07</v>
@@ -3835,7 +3839,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B88">
         <v>8.27</v>
@@ -3854,7 +3858,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B89">
         <v>8.2899999999999991</v>
@@ -3873,7 +3877,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B90">
         <v>8.3699999999999992</v>
@@ -3892,7 +3896,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B91">
         <v>8.3800000000000008</v>
@@ -3911,7 +3915,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B92">
         <v>8.42</v>
@@ -3930,7 +3934,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B93">
         <v>8.49</v>
@@ -3949,7 +3953,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B94">
         <v>8.5399999999999991</v>
@@ -3968,7 +3972,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95">
         <v>8.59</v>
@@ -3987,7 +3991,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B96">
         <v>8.6199999999999992</v>
@@ -4006,7 +4010,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B97">
         <v>8.67</v>
@@ -4025,7 +4029,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B98">
         <v>8.67</v>
@@ -4044,7 +4048,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B99">
         <v>8.68</v>
@@ -4063,7 +4067,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B100">
         <v>8.7200000000000006</v>
@@ -4082,7 +4086,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B101">
         <v>8.73</v>
@@ -4101,7 +4105,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B102">
         <v>8.73</v>
@@ -4120,7 +4124,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B103">
         <v>8.8699999999999992</v>
@@ -4139,7 +4143,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B104">
         <v>8.9</v>
@@ -4158,7 +4162,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B105">
         <v>8.91</v>
@@ -4177,7 +4181,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B106">
         <v>8.9499999999999993</v>
@@ -4196,7 +4200,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B107">
         <v>8.9499999999999993</v>
@@ -4215,7 +4219,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B108">
         <v>9.06</v>
@@ -4234,7 +4238,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B109">
         <v>9.1300000000000008</v>
@@ -4253,7 +4257,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B110">
         <v>9.19</v>
@@ -4272,7 +4276,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B111">
         <v>9.23</v>
@@ -4291,7 +4295,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B112">
         <v>9.26</v>
@@ -4310,7 +4314,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B113">
         <v>9.34</v>
@@ -4329,7 +4333,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B114">
         <v>9.3699999999999992</v>
@@ -4348,7 +4352,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B115">
         <v>9.3800000000000008</v>
@@ -4367,7 +4371,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B116">
         <v>9.39</v>
@@ -4386,7 +4390,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B117">
         <v>9.43</v>
@@ -4405,7 +4409,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B118">
         <v>9.4600000000000009</v>
@@ -4424,7 +4428,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B119">
         <v>9.51</v>
@@ -4443,7 +4447,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B120">
         <v>9.5500000000000007</v>
@@ -4462,7 +4466,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B121">
         <v>9.57</v>
@@ -4481,7 +4485,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B122">
         <v>9.65</v>
@@ -4500,7 +4504,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B123">
         <v>9.7899999999999991</v>
@@ -4519,7 +4523,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B124">
         <v>9.82</v>
@@ -4538,7 +4542,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B125">
         <v>10.07</v>
@@ -4557,7 +4561,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B126">
         <v>10.119999999999999</v>
@@ -4576,7 +4580,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B127">
         <v>10.14</v>
@@ -4595,7 +4599,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B128">
         <v>10.18</v>
@@ -4614,7 +4618,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B129">
         <v>10.18</v>
@@ -4633,7 +4637,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B130">
         <v>10.210000000000001</v>
@@ -4652,7 +4656,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B131">
         <v>10.32</v>
@@ -4671,7 +4675,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B132">
         <v>10.52</v>
@@ -4690,7 +4694,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B133">
         <v>10.54</v>
@@ -4709,7 +4713,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B134">
         <v>10.58</v>
@@ -4728,7 +4732,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B135">
         <v>10.77</v>
@@ -4747,7 +4751,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B136">
         <v>10.78</v>
@@ -4766,7 +4770,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B137">
         <v>10.78</v>
@@ -4785,7 +4789,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B138">
         <v>10.81</v>
@@ -4804,7 +4808,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B139">
         <v>10.82</v>
@@ -4823,7 +4827,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B140">
         <v>10.89</v>
@@ -4842,7 +4846,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B141">
         <v>11</v>
@@ -4861,7 +4865,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B142">
         <v>11.05</v>
@@ -4880,7 +4884,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B143">
         <v>11.09</v>
@@ -4899,7 +4903,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B144">
         <v>11.12</v>
@@ -4918,7 +4922,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B145">
         <v>11.19</v>
@@ -4937,7 +4941,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B146">
         <v>11.22</v>
@@ -4956,7 +4960,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B147">
         <v>11.34</v>
@@ -4975,7 +4979,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B148">
         <v>11.36</v>
@@ -4994,7 +4998,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B149">
         <v>11.36</v>
@@ -5013,7 +5017,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B150">
         <v>11.37</v>
@@ -5032,7 +5036,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B151">
         <v>11.44</v>
@@ -5051,7 +5055,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B152">
         <v>11.44</v>
@@ -5070,7 +5074,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B153">
         <v>11.52</v>
@@ -5089,7 +5093,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B154">
         <v>11.59</v>
@@ -5108,7 +5112,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B155">
         <v>11.65</v>
@@ -5127,7 +5131,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B156">
         <v>11.69</v>
@@ -5146,7 +5150,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B157">
         <v>11.76</v>
@@ -5165,7 +5169,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B158">
         <v>11.82</v>
@@ -5184,7 +5188,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B159">
         <v>11.91</v>
@@ -5203,7 +5207,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B160">
         <v>11.97</v>
@@ -5222,7 +5226,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B161">
         <v>12.01</v>
@@ -5241,7 +5245,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B162">
         <v>12.02</v>
@@ -5260,7 +5264,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B163">
         <v>12.11</v>
@@ -5279,7 +5283,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B164">
         <v>12.21</v>
@@ -5298,7 +5302,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B165">
         <v>12.22</v>
@@ -5317,7 +5321,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B166">
         <v>12.22</v>
@@ -5336,7 +5340,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B167">
         <v>12.3</v>
@@ -5355,7 +5359,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B168">
         <v>12.74</v>
@@ -5374,7 +5378,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B169">
         <v>12.74</v>
@@ -5393,7 +5397,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B170">
         <v>12.81</v>
@@ -5412,7 +5416,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B171">
         <v>12.94</v>
@@ -5431,7 +5435,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B172">
         <v>12.96</v>
@@ -5450,7 +5454,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B173">
         <v>12.99</v>
@@ -5469,7 +5473,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B174">
         <v>13.06</v>
@@ -5488,7 +5492,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B175">
         <v>13.13</v>
@@ -5507,7 +5511,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B176">
         <v>13.2</v>
@@ -5526,7 +5530,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B177">
         <v>13.21</v>
@@ -5545,7 +5549,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B178">
         <v>13.23</v>
@@ -5564,7 +5568,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B179">
         <v>13.33</v>
@@ -5583,7 +5587,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B180">
         <v>13.34</v>
@@ -5602,7 +5606,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B181">
         <v>13.36</v>
@@ -5621,7 +5625,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B182">
         <v>13.45</v>
@@ -5640,7 +5644,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B183">
         <v>13.52</v>
@@ -5659,7 +5663,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B184">
         <v>13.57</v>
@@ -5678,7 +5682,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B185">
         <v>13.61</v>
@@ -5697,7 +5701,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B186">
         <v>13.61</v>
@@ -5716,7 +5720,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B187">
         <v>13.62</v>
@@ -5735,7 +5739,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B188">
         <v>13.65</v>
@@ -5754,7 +5758,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B189">
         <v>13.69</v>
@@ -5773,7 +5777,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B190">
         <v>13.72</v>
@@ -5792,7 +5796,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B191">
         <v>13.77</v>
@@ -5811,7 +5815,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B192">
         <v>13.87</v>
@@ -5830,7 +5834,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B193">
         <v>13.88</v>
@@ -5849,7 +5853,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B194">
         <v>14.11</v>
@@ -5868,7 +5872,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B195">
         <v>14.11</v>
@@ -5887,7 +5891,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B196">
         <v>14.12</v>
@@ -5906,7 +5910,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B197">
         <v>14.29</v>
@@ -5925,7 +5929,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B198">
         <v>14.32</v>
@@ -5944,7 +5948,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B199">
         <v>14.39</v>
@@ -5963,7 +5967,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B200">
         <v>14.6</v>
@@ -5982,7 +5986,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B201">
         <v>15.07</v>
@@ -6001,7 +6005,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B202">
         <v>15.08</v>
@@ -6020,7 +6024,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B203">
         <v>15.09</v>
@@ -6039,7 +6043,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B204">
         <v>15.09</v>
@@ -6058,7 +6062,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B205">
         <v>15.13</v>
@@ -6077,7 +6081,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B206">
         <v>15.28</v>
@@ -6096,7 +6100,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B207">
         <v>15.29</v>
@@ -6115,7 +6119,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B208">
         <v>15.32</v>
@@ -6134,7 +6138,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B209">
         <v>15.36</v>
@@ -6153,7 +6157,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B210">
         <v>15.42</v>
@@ -6172,7 +6176,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B211">
         <v>15.55</v>
@@ -6191,7 +6195,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B212">
         <v>15.62</v>
@@ -6210,7 +6214,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B213">
         <v>15.65</v>
@@ -6229,7 +6233,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B214">
         <v>15.69</v>
@@ -6248,7 +6252,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B215">
         <v>15.77</v>
@@ -6267,7 +6271,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B216">
         <v>15.8</v>
@@ -6286,7 +6290,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B217">
         <v>15.82</v>
@@ -6305,7 +6309,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B218">
         <v>15.9</v>
@@ -6324,7 +6328,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B219">
         <v>16.29</v>
@@ -6343,7 +6347,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B220">
         <v>16.3</v>
@@ -6362,7 +6366,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B221">
         <v>16.309999999999999</v>
@@ -6381,7 +6385,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B222">
         <v>16.350000000000001</v>
@@ -6400,7 +6404,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B223">
         <v>16.38</v>
@@ -6419,7 +6423,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B224">
         <v>16.420000000000002</v>
@@ -6438,7 +6442,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B225">
         <v>16.510000000000002</v>
@@ -6457,7 +6461,7 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B226">
         <v>16.52</v>
@@ -6476,7 +6480,7 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B227">
         <v>16.55</v>
@@ -6495,7 +6499,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B228">
         <v>16.579999999999998</v>
@@ -6514,7 +6518,7 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B229">
         <v>16.59</v>
@@ -6533,7 +6537,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B230">
         <v>16.62</v>
@@ -6552,7 +6556,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B231">
         <v>16.690000000000001</v>
@@ -6571,7 +6575,7 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B232">
         <v>16.72</v>
@@ -6590,7 +6594,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B233">
         <v>16.8</v>
@@ -6628,7 +6632,7 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B235">
         <v>17.11</v>
@@ -6647,7 +6651,7 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B236">
         <v>17.32</v>
@@ -6666,7 +6670,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B237">
         <v>17.34</v>
@@ -6685,7 +6689,7 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B238">
         <v>17.47</v>
@@ -6704,7 +6708,7 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B239">
         <v>17.489999999999998</v>
@@ -6723,7 +6727,7 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B240">
         <v>17.57</v>
@@ -6742,7 +6746,7 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B241">
         <v>17.62</v>
@@ -6761,7 +6765,7 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B242">
         <v>18.010000000000002</v>
@@ -6780,7 +6784,7 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B243">
         <v>18.03</v>
@@ -6799,7 +6803,7 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B244">
         <v>18.04</v>
@@ -6818,7 +6822,7 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B245">
         <v>18.09</v>
@@ -6837,7 +6841,7 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B246">
         <v>18.100000000000001</v>
@@ -6856,7 +6860,7 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B247">
         <v>18.14</v>
@@ -6875,7 +6879,7 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B248">
         <v>18.47</v>
@@ -6894,7 +6898,7 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B249">
         <v>18.510000000000002</v>
@@ -6913,7 +6917,7 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B250">
         <v>18.559999999999999</v>
@@ -6932,7 +6936,7 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B251">
         <v>18.63</v>
@@ -6951,7 +6955,7 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B252">
         <v>19.14</v>
@@ -6970,7 +6974,7 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B253">
         <v>19.2</v>
@@ -6989,7 +6993,7 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B254">
         <v>19.27</v>
@@ -7008,7 +7012,7 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B255">
         <v>19.38</v>
@@ -7027,7 +7031,7 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B256">
         <v>19.43</v>
@@ -7046,7 +7050,7 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B257">
         <v>19.45</v>
@@ -7065,7 +7069,7 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B258">
         <v>19.47</v>
@@ -7084,7 +7088,7 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B259">
         <v>19.95</v>
@@ -7103,7 +7107,7 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B260">
         <v>20.079999999999998</v>
@@ -7122,7 +7126,7 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B261">
         <v>20.190000000000001</v>
@@ -7141,7 +7145,7 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B262">
         <v>20.29</v>
@@ -7160,7 +7164,7 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B263">
         <v>20.36</v>
@@ -7198,7 +7202,7 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B265">
         <v>20.61</v>
@@ -7217,7 +7221,7 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B266">
         <v>20.77</v>
@@ -7236,7 +7240,7 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B267">
         <v>20.86</v>
@@ -7255,7 +7259,7 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B268">
         <v>21.24</v>
@@ -7274,7 +7278,7 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B269">
         <v>21.27</v>
@@ -7293,7 +7297,7 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B270">
         <v>21.31</v>
@@ -7312,7 +7316,7 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B271">
         <v>21.63</v>
@@ -7331,7 +7335,7 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B272">
         <v>21.64</v>
@@ -7350,7 +7354,7 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B273">
         <v>21.73</v>
@@ -7369,7 +7373,7 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B274">
         <v>21.85</v>
@@ -7388,7 +7392,7 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B275">
         <v>22.09</v>
@@ -7407,7 +7411,7 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B276">
         <v>22.38</v>
@@ -7426,7 +7430,7 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B277">
         <v>22.39</v>
@@ -7445,7 +7449,7 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B278">
         <v>22.52</v>
@@ -7464,7 +7468,7 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B279">
         <v>22.54</v>
@@ -7483,7 +7487,7 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B280">
         <v>22.61</v>
@@ -7502,7 +7506,7 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B281">
         <v>22.61</v>
@@ -7521,7 +7525,7 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B282">
         <v>22.65</v>
@@ -7540,7 +7544,7 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B283">
         <v>22.83</v>
@@ -7559,7 +7563,7 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B284">
         <v>23.16</v>
@@ -7578,7 +7582,7 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B285">
         <v>23.25</v>
@@ -7597,7 +7601,7 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B286">
         <v>23.41</v>
@@ -7616,7 +7620,7 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B287">
         <v>23.45</v>
@@ -7635,7 +7639,7 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B288">
         <v>23.57</v>
@@ -7654,7 +7658,7 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B289">
         <v>23.75</v>
@@ -7673,7 +7677,7 @@
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B290">
         <v>23.77</v>
@@ -7692,7 +7696,7 @@
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>4</v>
+        <v>357</v>
       </c>
       <c r="B291">
         <v>23.88</v>
@@ -7711,7 +7715,7 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B292">
         <v>23.9</v>
@@ -7730,7 +7734,7 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B293">
         <v>23.93</v>
@@ -7749,7 +7753,7 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B294">
         <v>23.98</v>
@@ -7768,7 +7772,7 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B295">
         <v>24.1</v>
@@ -7787,7 +7791,7 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B296">
         <v>24.18</v>
@@ -7806,7 +7810,7 @@
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B297">
         <v>24.22</v>
@@ -7825,7 +7829,7 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B298">
         <v>24.44</v>
@@ -7844,7 +7848,7 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B299">
         <v>24.51</v>
@@ -7863,7 +7867,7 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B300">
         <v>24.54</v>
@@ -7882,7 +7886,7 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B301">
         <v>24.6</v>
@@ -7901,7 +7905,7 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B302">
         <v>24.64</v>
@@ -7920,7 +7924,7 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B303">
         <v>24.65</v>
@@ -7939,7 +7943,7 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B304">
         <v>24.69</v>
@@ -7958,7 +7962,7 @@
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B305">
         <v>24.84</v>
@@ -7977,7 +7981,7 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B306">
         <v>24.95</v>
@@ -7996,7 +8000,7 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B307">
         <v>25.04</v>
@@ -8015,7 +8019,7 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B308">
         <v>25.39</v>
@@ -8034,7 +8038,7 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B309">
         <v>25.44</v>
@@ -8053,7 +8057,7 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B310">
         <v>25.49</v>
@@ -8072,7 +8076,7 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B311">
         <v>25.63</v>
@@ -8091,7 +8095,7 @@
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B312">
         <v>25.83</v>
@@ -8110,7 +8114,7 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B313">
         <v>26.3</v>
@@ -8129,7 +8133,7 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B314">
         <v>26.34</v>
@@ -8148,7 +8152,7 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B315">
         <v>26.7</v>
@@ -8167,7 +8171,7 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B316">
         <v>27.74</v>
@@ -8215,10 +8219,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -10631,7 +10635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC484A4-F4B1-4211-8858-3AD160FDAD22}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -10644,19 +10648,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B4" s="1">
         <v>0.97847749700374798</v>
@@ -10664,7 +10668,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" s="1">
         <v>0.9574182121427196</v>
@@ -10672,7 +10676,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="5">
         <v>0.95727532023715833</v>
@@ -10680,7 +10684,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B7" s="1">
         <v>1.2451167561865917</v>
@@ -10688,7 +10692,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B8" s="2">
         <v>300</v>
@@ -10696,30 +10700,30 @@
     </row>
     <row r="10" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -10739,7 +10743,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B13" s="1">
         <v>298</v>
@@ -10753,7 +10757,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="H13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I13" s="6">
         <f>SQRT(D13)</f>
@@ -10762,7 +10766,7 @@
     </row>
     <row r="14" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B14" s="2">
         <v>299</v>
@@ -10778,33 +10782,33 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B17" s="1">
         <v>1.7779272265709221</v>
@@ -10833,7 +10837,7 @@
     </row>
     <row r="18" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B18" s="2">
         <v>0.86773417211758253</v>
@@ -10881,22 +10885,22 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B4" s="1">
         <v>12.57916666666666</v>
@@ -10907,7 +10911,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="1">
         <v>46.139153483835187</v>
@@ -10918,7 +10922,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B6" s="1">
         <v>300</v>
@@ -10929,7 +10933,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B7" s="1">
         <v>299</v>
@@ -10940,7 +10944,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B8" s="5">
         <v>1.2715348949042349</v>
@@ -10949,7 +10953,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B9" s="1">
         <v>1.9099334878920737E-2</v>
@@ -10958,7 +10962,7 @@
     </row>
     <row r="10" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B10" s="2">
         <v>1.209916742593254</v>

</xml_diff>